<commit_message>
Nb obs per group
</commit_message>
<xml_diff>
--- a/data/RawData/ObsData/2001-2009/01-06-2004.xlsx
+++ b/data/RawData/ObsData/2001-2009/01-06-2004.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aponchon\Nextcloud\Aurore Ponchon\Projects\Golden Lion Tamarins Brazil\Analysis\GoldenLionTamarins\data\RawData\pdfData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aponchon\Nextcloud\Aurore Ponchon\Projects\Golden Lion Tamarins Brazil\Analysis\GoldenLionTamarins\data\RawData\ObsData\2001-2009\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A391D075-EB83-4B03-8B5A-68615BFFDB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F37270-CBE0-4F19-82F7-406E273CA346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="675" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="1295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2970" uniqueCount="1294">
   <si>
     <t>Mico</t>
   </si>
@@ -7713,17 +7713,6 @@
         <family val="1"/>
       </rPr>
       <t>T4-PE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF978C99"/>
-        <rFont val="Amasis MT Pro"/>
-        <family val="1"/>
-      </rPr>
-      <t>'</t>
     </r>
   </si>
   <si>
@@ -8735,7 +8724,7 @@
     <numFmt numFmtId="164" formatCode="00000"/>
     <numFmt numFmtId="165" formatCode="000"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -8932,12 +8921,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF181515"/>
-      <name val="Amasis MT Pro"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF978C99"/>
       <name val="Amasis MT Pro"/>
       <family val="1"/>
     </font>
@@ -9379,10 +9362,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="36" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9460,10 +9443,10 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="38" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="37" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="1" fontId="38" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="37" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9613,7 +9596,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="41" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="40" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10686,8 +10669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N103" sqref="N103:N296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -10711,7 +10694,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="96" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="83"/>
@@ -10759,7 +10742,7 @@
         <v>6</v>
       </c>
       <c r="J3" s="61" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K3" s="61" t="s">
         <v>7</v>
@@ -11012,7 +10995,7 @@
     <row r="10" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="86"/>
       <c r="B10" s="86" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="C10" s="86" t="s">
         <v>21</v>
@@ -11047,13 +11030,13 @@
     <row r="11" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="86"/>
       <c r="B11" s="86" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="C11" s="86" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D11" s="86" t="s">
         <v>1230</v>
-      </c>
-      <c r="D11" s="86" t="s">
-        <v>1231</v>
       </c>
       <c r="E11" s="86" t="s">
         <v>22</v>
@@ -11074,13 +11057,13 @@
     <row r="12" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="86"/>
       <c r="B12" s="86" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="C12" s="86" t="s">
         <v>366</v>
       </c>
       <c r="D12" s="86" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="E12" s="86" t="s">
         <v>22</v>
@@ -11154,13 +11137,13 @@
     <row r="14" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="86"/>
       <c r="B14" s="86" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C14" s="86" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="86" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="E14" s="86" t="s">
         <v>22</v>
@@ -11211,13 +11194,13 @@
       <c r="H15" s="3"/>
       <c r="I15" s="61"/>
       <c r="J15" s="61" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="K15" s="61" t="s">
         <v>380</v>
       </c>
       <c r="L15" s="61" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="M15" s="61" t="s">
         <v>14</v>
@@ -11248,11 +11231,11 @@
       <c r="H16" s="3"/>
       <c r="I16" s="61"/>
       <c r="J16" s="61" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="K16" s="61"/>
       <c r="L16" s="61" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="M16" s="61" t="s">
         <v>14</v>
@@ -11283,11 +11266,11 @@
       <c r="H17" s="5"/>
       <c r="I17" s="61"/>
       <c r="J17" s="61" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="K17" s="61"/>
       <c r="L17" s="61" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="M17" s="61" t="s">
         <v>22</v>
@@ -11345,11 +11328,11 @@
       <c r="H19" s="1"/>
       <c r="I19" s="61"/>
       <c r="J19" s="65" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="K19" s="61"/>
       <c r="L19" s="65" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="M19" s="61" t="s">
         <v>22</v>
@@ -11364,7 +11347,7 @@
         <v>95</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C20" s="65" t="s">
         <v>673</v>
@@ -11376,7 +11359,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="G20" s="69">
         <v>4867</v>
@@ -11384,11 +11367,11 @@
       <c r="H20" s="1"/>
       <c r="I20" s="61"/>
       <c r="J20" s="61" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="K20" s="61"/>
       <c r="L20" s="61" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="M20" s="61" t="s">
         <v>22</v>
@@ -11718,11 +11701,11 @@
       <c r="H30" s="3"/>
       <c r="I30" s="65"/>
       <c r="J30" s="65" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="K30" s="65"/>
       <c r="L30" s="65" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="M30" s="65" t="s">
         <v>22</v>
@@ -11747,11 +11730,11 @@
       <c r="H31" s="5"/>
       <c r="I31" s="65"/>
       <c r="J31" s="65" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="K31" s="65"/>
       <c r="L31" s="65" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="M31" s="65" t="s">
         <v>22</v>
@@ -11772,11 +11755,11 @@
       <c r="H32" s="5"/>
       <c r="I32" s="65"/>
       <c r="J32" s="65" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="K32" s="65"/>
       <c r="L32" s="65" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="M32" s="65" t="s">
         <v>22</v>
@@ -11892,13 +11875,13 @@
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="86"/>
       <c r="B36" s="86" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C36" s="86" t="s">
         <v>1236</v>
       </c>
-      <c r="C36" s="86" t="s">
-        <v>1237</v>
-      </c>
       <c r="D36" s="86" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="E36" s="86" t="s">
         <v>14</v>
@@ -11926,9 +11909,7 @@
       <c r="E37" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="86" t="s">
-        <v>130</v>
-      </c>
+      <c r="F37" s="86"/>
       <c r="G37" s="86"/>
       <c r="H37" s="3"/>
       <c r="I37" s="86" t="s">
@@ -12023,9 +12004,7 @@
       <c r="C40" s="86"/>
       <c r="D40" s="86"/>
       <c r="E40" s="86"/>
-      <c r="F40" s="86" t="s">
-        <v>130</v>
-      </c>
+      <c r="F40" s="86"/>
       <c r="G40" s="86"/>
       <c r="H40" s="3"/>
       <c r="I40" s="113"/>
@@ -12604,7 +12583,7 @@
         <v>6</v>
       </c>
       <c r="J57" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K57" s="86" t="s">
         <v>224</v>
@@ -12688,7 +12667,7 @@
         <v>6</v>
       </c>
       <c r="B60" s="61" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C60" s="61" t="s">
         <v>224</v>
@@ -12779,9 +12758,7 @@
       <c r="E62" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="F62" s="61" t="s">
-        <v>130</v>
-      </c>
+      <c r="F62" s="61"/>
       <c r="G62" s="61"/>
       <c r="H62" s="24"/>
       <c r="O62" s="72"/>
@@ -12859,13 +12836,13 @@
     <row r="65" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="65"/>
       <c r="B65" s="61" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="C65" s="61" t="s">
         <v>128</v>
       </c>
       <c r="D65" s="61" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="E65" s="61" t="s">
         <v>14</v>
@@ -12935,13 +12912,13 @@
     <row r="67" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="61"/>
       <c r="B67" s="65" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="C67" s="65" t="s">
         <v>618</v>
       </c>
       <c r="D67" s="65" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="E67" s="65" t="s">
         <v>14</v>
@@ -13009,13 +12986,13 @@
     <row r="69" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="61"/>
       <c r="B69" s="61" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C69" s="61" t="s">
         <v>132</v>
       </c>
       <c r="D69" s="61" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="E69" s="61" t="s">
         <v>22</v>
@@ -13114,7 +13091,7 @@
     <row r="72" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="61"/>
       <c r="B72" s="61" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="C72" s="61"/>
       <c r="D72" s="61"/>
@@ -13609,17 +13586,17 @@
         <v>363</v>
       </c>
       <c r="J87" s="86" t="s">
+        <v>1242</v>
+      </c>
+      <c r="K87" s="86" t="s">
         <v>1243</v>
-      </c>
-      <c r="K87" s="86" t="s">
-        <v>1244</v>
       </c>
       <c r="L87" s="113"/>
       <c r="M87" s="86" t="s">
         <v>171</v>
       </c>
       <c r="N87" s="86" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="O87" s="115">
         <v>4366</v>
@@ -13647,20 +13624,20 @@
       <c r="G88" s="113"/>
       <c r="H88" s="3"/>
       <c r="I88" s="86" t="s">
+        <v>1245</v>
+      </c>
+      <c r="J88" s="86" t="s">
         <v>1246</v>
       </c>
-      <c r="J88" s="86" t="s">
+      <c r="K88" s="86" t="s">
         <v>1247</v>
-      </c>
-      <c r="K88" s="86" t="s">
-        <v>1248</v>
       </c>
       <c r="L88" s="113"/>
       <c r="M88" s="86" t="s">
         <v>171</v>
       </c>
       <c r="N88" s="86" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="O88" s="113"/>
     </row>
@@ -13930,7 +13907,7 @@
     </row>
     <row r="97" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="44" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="B97" s="86" t="s">
         <v>340</v>
@@ -14152,9 +14129,7 @@
       <c r="M103" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="N103" s="61" t="s">
-        <v>130</v>
-      </c>
+      <c r="N103" s="61"/>
       <c r="O103" s="61"/>
     </row>
     <row r="104" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14687,7 +14662,7 @@
       <c r="G122" s="61"/>
       <c r="H122" s="35"/>
       <c r="I122" s="90" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="J122" s="90" t="s">
         <v>492</v>
@@ -15455,7 +15430,7 @@
       <c r="G147" s="86"/>
       <c r="H147" s="35"/>
       <c r="I147" s="61" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="J147" s="61" t="s">
         <v>478</v>
@@ -15501,7 +15476,7 @@
     </row>
     <row r="149" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="86" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B149" s="97"/>
       <c r="C149" s="86"/>
@@ -15563,7 +15538,7 @@
         <v>14</v>
       </c>
       <c r="N150" s="66" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="O150" s="65"/>
     </row>
@@ -15588,7 +15563,7 @@
       <c r="H151" s="35"/>
       <c r="I151" s="69"/>
       <c r="J151" s="118" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K151" s="61"/>
       <c r="L151" s="118"/>
@@ -15619,7 +15594,7 @@
       <c r="H152" s="35"/>
       <c r="I152" s="69"/>
       <c r="J152" s="119" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="K152" s="61"/>
       <c r="L152" s="119"/>
@@ -15682,7 +15657,7 @@
         <v>6</v>
       </c>
       <c r="B155" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C155" s="86" t="s">
         <v>224</v>
@@ -15732,9 +15707,7 @@
       <c r="E156" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="F156" s="86" t="s">
-        <v>130</v>
-      </c>
+      <c r="F156" s="86"/>
       <c r="G156" s="86">
         <v>4899</v>
       </c>
@@ -15875,7 +15848,7 @@
         <v>6</v>
       </c>
       <c r="J160" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K160" s="86" t="s">
         <v>224</v>
@@ -15993,7 +15966,7 @@
         <v>6</v>
       </c>
       <c r="B164" s="61" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C164" s="61" t="s">
         <v>224</v>
@@ -16890,9 +16863,7 @@
       <c r="E190" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="F190" s="86" t="s">
-        <v>130</v>
-      </c>
+      <c r="F190" s="86"/>
       <c r="G190" s="87">
         <v>4289</v>
       </c>
@@ -17105,13 +17076,13 @@
         <v>464</v>
       </c>
       <c r="J197" s="111" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="K197" s="111" t="s">
         <v>544</v>
       </c>
       <c r="L197" s="111" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="M197" s="111" t="s">
         <v>22</v>
@@ -17194,7 +17165,7 @@
       <c r="G200" s="86"/>
       <c r="H200" s="24"/>
       <c r="I200" s="86" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="J200" s="86"/>
       <c r="K200" s="86"/>
@@ -17218,7 +17189,7 @@
         <v>508</v>
       </c>
       <c r="J201" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K201" s="86" t="s">
         <v>509</v>
@@ -17248,7 +17219,7 @@
       <c r="G202" s="86"/>
       <c r="H202" s="120"/>
       <c r="I202" s="121" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="J202" s="86" t="s">
         <v>719</v>
@@ -17515,7 +17486,7 @@
         <v>6</v>
       </c>
       <c r="B211" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C211" s="86" t="s">
         <v>224</v>
@@ -17568,7 +17539,7 @@
         <v>508</v>
       </c>
       <c r="J212" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K212" s="86" t="s">
         <v>509</v>
@@ -18327,13 +18298,13 @@
       <c r="H234" s="8"/>
       <c r="I234" s="113"/>
       <c r="J234" s="86" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="K234" s="86" t="s">
         <v>360</v>
       </c>
       <c r="L234" s="86" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M234" s="86" t="s">
         <v>22</v>
@@ -18438,13 +18409,13 @@
       <c r="H237" s="6"/>
       <c r="I237" s="113"/>
       <c r="J237" s="123" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="K237" s="123" t="s">
         <v>32</v>
       </c>
       <c r="L237" s="123" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="M237" s="130" t="s">
         <v>500</v>
@@ -18906,7 +18877,7 @@
         <v>508</v>
       </c>
       <c r="J252" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K252" s="86" t="s">
         <v>851</v>
@@ -19289,7 +19260,7 @@
         <v>6</v>
       </c>
       <c r="B264" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C264" s="86" t="s">
         <v>224</v>
@@ -19931,9 +19902,7 @@
       <c r="M281" s="86" t="s">
         <v>527</v>
       </c>
-      <c r="N281" s="86" t="s">
-        <v>507</v>
-      </c>
+      <c r="N281" s="86"/>
       <c r="O281" s="113"/>
     </row>
     <row r="282" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -19956,9 +19925,7 @@
       <c r="M282" s="86" t="s">
         <v>502</v>
       </c>
-      <c r="N282" s="86" t="s">
-        <v>507</v>
-      </c>
+      <c r="N282" s="86"/>
       <c r="O282" s="113"/>
     </row>
     <row r="283" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -20241,13 +20208,13 @@
         <v>919</v>
       </c>
       <c r="B291" s="65" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="C291" s="65" t="s">
         <v>593</v>
       </c>
       <c r="D291" s="65" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="E291" s="65" t="s">
         <v>22</v>
@@ -20274,13 +20241,13 @@
     <row r="292" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="61"/>
       <c r="B292" s="61" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="C292" s="61" t="s">
         <v>597</v>
       </c>
       <c r="D292" s="61" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="E292" s="61" t="s">
         <v>14</v>
@@ -20328,13 +20295,13 @@
     <row r="294" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="61"/>
       <c r="B294" s="61" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C294" s="61" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="D294" s="61" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="E294" s="61" t="s">
         <v>22</v>
@@ -20357,13 +20324,13 @@
     <row r="295" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="61"/>
       <c r="B295" s="65" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C295" s="65" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="D295" s="65" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="E295" s="65" t="s">
         <v>14</v>
@@ -20425,9 +20392,7 @@
       <c r="M296" s="86" t="s">
         <v>502</v>
       </c>
-      <c r="N296" s="86" t="s">
-        <v>507</v>
-      </c>
+      <c r="N296" s="86"/>
       <c r="O296" s="113"/>
     </row>
     <row r="297" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20659,7 +20624,7 @@
       <c r="G304" s="86"/>
       <c r="H304" s="19"/>
       <c r="I304" s="86" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="J304" s="97"/>
       <c r="K304" s="113"/>
@@ -20852,7 +20817,7 @@
         <v>6</v>
       </c>
       <c r="B310" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C310" s="86" t="s">
         <v>981</v>
@@ -20985,22 +20950,22 @@
     </row>
     <row r="314" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A314" s="86" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B314" s="86" t="s">
         <v>1253</v>
       </c>
-      <c r="B314" s="86" t="s">
+      <c r="C314" s="86" t="s">
         <v>1254</v>
       </c>
-      <c r="C314" s="86" t="s">
+      <c r="D314" s="86" t="s">
+        <v>1253</v>
+      </c>
+      <c r="E314" s="130" t="s">
         <v>1255</v>
       </c>
-      <c r="D314" s="86" t="s">
-        <v>1254</v>
-      </c>
-      <c r="E314" s="130" t="s">
+      <c r="F314" s="86" t="s">
         <v>1256</v>
-      </c>
-      <c r="F314" s="86" t="s">
-        <v>1257</v>
       </c>
       <c r="G314" s="113"/>
       <c r="H314" s="43"/>
@@ -21015,13 +20980,13 @@
     <row r="315" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A315" s="113"/>
       <c r="B315" s="86" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C315" s="86" t="s">
         <v>1258</v>
       </c>
-      <c r="C315" s="86" t="s">
-        <v>1259</v>
-      </c>
       <c r="D315" s="86" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="E315" s="86" t="s">
         <v>924</v>
@@ -21056,19 +21021,19 @@
     <row r="316" spans="1:15" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A316" s="113"/>
       <c r="B316" s="86" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C316" s="86" t="s">
         <v>1260</v>
       </c>
-      <c r="C316" s="86" t="s">
+      <c r="D316" s="130" t="s">
         <v>1261</v>
       </c>
-      <c r="D316" s="130" t="s">
+      <c r="E316" s="130" t="s">
+        <v>1255</v>
+      </c>
+      <c r="F316" s="86" t="s">
         <v>1262</v>
-      </c>
-      <c r="E316" s="130" t="s">
-        <v>1256</v>
-      </c>
-      <c r="F316" s="86" t="s">
-        <v>1263</v>
       </c>
       <c r="G316" s="113"/>
       <c r="H316" s="43"/>
@@ -21093,19 +21058,19 @@
     <row r="317" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A317" s="113"/>
       <c r="B317" s="130" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C317" s="86" t="s">
         <v>1264</v>
       </c>
-      <c r="C317" s="86" t="s">
+      <c r="D317" s="86" t="s">
         <v>1265</v>
-      </c>
-      <c r="D317" s="86" t="s">
-        <v>1266</v>
       </c>
       <c r="E317" s="86" t="s">
         <v>922</v>
       </c>
       <c r="F317" s="86" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="G317" s="113"/>
       <c r="H317" s="43"/>
@@ -21130,19 +21095,19 @@
     <row r="318" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A318" s="113"/>
       <c r="B318" s="86" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C318" s="86" t="s">
         <v>1267</v>
       </c>
-      <c r="C318" s="86" t="s">
-        <v>1268</v>
-      </c>
       <c r="D318" s="86" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="E318" s="86" t="s">
         <v>922</v>
       </c>
       <c r="F318" s="86" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="G318" s="113"/>
       <c r="H318" s="43"/>
@@ -21167,19 +21132,19 @@
     <row r="319" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A319" s="113"/>
       <c r="B319" s="86" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C319" s="86" t="s">
         <v>1270</v>
       </c>
-      <c r="C319" s="86" t="s">
-        <v>1271</v>
-      </c>
       <c r="D319" s="86" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="E319" s="130" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="F319" s="86" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="G319" s="113"/>
       <c r="H319" s="43"/>
@@ -21204,13 +21169,13 @@
     <row r="320" spans="1:15" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="113"/>
       <c r="B320" s="86" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C320" s="86" t="s">
         <v>1272</v>
       </c>
-      <c r="C320" s="86" t="s">
-        <v>1273</v>
-      </c>
       <c r="D320" s="86" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="E320" s="86" t="s">
         <v>922</v>
@@ -21235,13 +21200,13 @@
     <row r="321" spans="1:15" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A321" s="113"/>
       <c r="B321" s="86" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C321" s="86" t="s">
         <v>1274</v>
       </c>
-      <c r="C321" s="86" t="s">
-        <v>1275</v>
-      </c>
       <c r="D321" s="86" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="E321" s="86" t="s">
         <v>922</v>
@@ -21289,9 +21254,7 @@
       <c r="E323" s="61" t="s">
         <v>924</v>
       </c>
-      <c r="F323" s="61" t="s">
-        <v>1006</v>
-      </c>
+      <c r="F323" s="61"/>
       <c r="G323" s="69"/>
       <c r="H323" s="43"/>
       <c r="I323" s="133" t="s">
@@ -22257,7 +22220,7 @@
       <c r="G351" s="61"/>
       <c r="H351" s="46"/>
       <c r="I351" s="86" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="J351" s="97"/>
       <c r="K351" s="113"/>
@@ -22289,19 +22252,19 @@
         <v>6</v>
       </c>
       <c r="J352" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K352" s="86" t="s">
+        <v>1184</v>
+      </c>
+      <c r="L352" s="86" t="s">
         <v>1185</v>
       </c>
-      <c r="L352" s="86" t="s">
+      <c r="M352" s="86" t="s">
         <v>1186</v>
       </c>
-      <c r="M352" s="86" t="s">
+      <c r="N352" s="86" t="s">
         <v>1187</v>
-      </c>
-      <c r="N352" s="86" t="s">
-        <v>1188</v>
       </c>
       <c r="O352" s="97" t="s">
         <v>228</v>
@@ -22327,13 +22290,13 @@
       <c r="G353" s="65"/>
       <c r="H353" s="55"/>
       <c r="I353" s="143" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="J353" s="86" t="s">
+        <v>1188</v>
+      </c>
+      <c r="K353" s="86" t="s">
         <v>1189</v>
-      </c>
-      <c r="K353" s="86" t="s">
-        <v>1190</v>
       </c>
       <c r="L353" s="86" t="s">
         <v>199</v>
@@ -22359,13 +22322,13 @@
       <c r="H354" s="24"/>
       <c r="I354" s="113"/>
       <c r="J354" s="143" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="K354" s="143" t="s">
         <v>643</v>
       </c>
       <c r="L354" s="86" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="M354" s="86" t="s">
         <v>1120</v>
@@ -22384,10 +22347,10 @@
       <c r="H355" s="147"/>
       <c r="I355" s="113"/>
       <c r="J355" s="86" t="s">
+        <v>1190</v>
+      </c>
+      <c r="K355" s="86" t="s">
         <v>1191</v>
-      </c>
-      <c r="K355" s="86" t="s">
-        <v>1192</v>
       </c>
       <c r="L355" s="139">
         <v>461</v>
@@ -22396,7 +22359,7 @@
         <v>1119</v>
       </c>
       <c r="N355" s="86" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="O355" s="97"/>
     </row>
@@ -22423,10 +22386,10 @@
       <c r="H356" s="148"/>
       <c r="I356" s="113"/>
       <c r="J356" s="86" t="s">
+        <v>1193</v>
+      </c>
+      <c r="K356" s="86" t="s">
         <v>1194</v>
-      </c>
-      <c r="K356" s="86" t="s">
-        <v>1195</v>
       </c>
       <c r="L356" s="139">
         <v>514</v>
@@ -22435,7 +22398,7 @@
         <v>1120</v>
       </c>
       <c r="N356" s="86" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="O356" s="97"/>
     </row>
@@ -22454,13 +22417,13 @@
       <c r="H357" s="148"/>
       <c r="I357" s="113"/>
       <c r="J357" s="86" t="s">
+        <v>1196</v>
+      </c>
+      <c r="K357" s="86" t="s">
         <v>1197</v>
       </c>
-      <c r="K357" s="86" t="s">
-        <v>1198</v>
-      </c>
       <c r="L357" s="86" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="M357" s="86" t="s">
         <v>1119</v>
@@ -22491,13 +22454,13 @@
       <c r="H358" s="148"/>
       <c r="I358" s="113"/>
       <c r="J358" s="86" t="s">
+        <v>1198</v>
+      </c>
+      <c r="K358" s="86" t="s">
         <v>1199</v>
       </c>
-      <c r="K358" s="86" t="s">
-        <v>1200</v>
-      </c>
       <c r="L358" s="86" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="M358" s="86" t="s">
         <v>1120</v>
@@ -22528,13 +22491,13 @@
       <c r="H359" s="148"/>
       <c r="I359" s="113"/>
       <c r="J359" s="86" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="K359" s="86" t="s">
         <v>1146</v>
       </c>
       <c r="L359" s="86" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="M359" s="86" t="s">
         <v>1120</v>
@@ -22568,13 +22531,13 @@
     <row r="361" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A361" s="155"/>
       <c r="B361" s="86" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C361" s="86" t="s">
         <v>125</v>
       </c>
       <c r="D361" s="86" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="E361" s="86" t="s">
         <v>22</v>
@@ -22585,16 +22548,16 @@
       <c r="G361" s="97"/>
       <c r="H361" s="148"/>
       <c r="I361" s="61" t="s">
+        <v>1201</v>
+      </c>
+      <c r="J361" s="61" t="s">
         <v>1202</v>
       </c>
-      <c r="J361" s="61" t="s">
+      <c r="K361" s="61" t="s">
         <v>1203</v>
       </c>
-      <c r="K361" s="61" t="s">
-        <v>1204</v>
-      </c>
       <c r="L361" s="61" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="M361" s="61" t="s">
         <v>1119</v>
@@ -22612,13 +22575,13 @@
       <c r="G362" s="75"/>
       <c r="I362" s="69"/>
       <c r="J362" s="61" t="s">
+        <v>1204</v>
+      </c>
+      <c r="K362" s="61" t="s">
         <v>1205</v>
       </c>
-      <c r="K362" s="61" t="s">
-        <v>1206</v>
-      </c>
       <c r="L362" s="61" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="M362" s="61" t="s">
         <v>1120</v>
@@ -22639,13 +22602,13 @@
       <c r="H363" s="22"/>
       <c r="I363" s="69"/>
       <c r="J363" s="61" t="s">
+        <v>1206</v>
+      </c>
+      <c r="K363" s="61" t="s">
         <v>1207</v>
       </c>
-      <c r="K363" s="61" t="s">
-        <v>1208</v>
-      </c>
       <c r="L363" s="61" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="M363" s="61" t="s">
         <v>1119</v>
@@ -22658,7 +22621,7 @@
         <v>6</v>
       </c>
       <c r="B364" s="86" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C364" s="86" t="s">
         <v>1141</v>
@@ -22678,10 +22641,10 @@
       <c r="H364" s="57"/>
       <c r="I364" s="69"/>
       <c r="J364" s="61" t="s">
+        <v>1208</v>
+      </c>
+      <c r="K364" s="61" t="s">
         <v>1209</v>
-      </c>
-      <c r="K364" s="61" t="s">
-        <v>1210</v>
       </c>
       <c r="L364" s="142">
         <v>460</v>
@@ -22715,13 +22678,13 @@
       <c r="H365" s="57"/>
       <c r="I365" s="69"/>
       <c r="J365" s="61" t="s">
+        <v>1210</v>
+      </c>
+      <c r="K365" s="61" t="s">
         <v>1211</v>
       </c>
-      <c r="K365" s="61" t="s">
-        <v>1212</v>
-      </c>
       <c r="L365" s="61" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="M365" s="61" t="s">
         <v>1119</v>
@@ -22748,13 +22711,13 @@
       <c r="H366" s="57"/>
       <c r="I366" s="69"/>
       <c r="J366" s="61" t="s">
+        <v>1212</v>
+      </c>
+      <c r="K366" s="61" t="s">
         <v>1213</v>
       </c>
-      <c r="K366" s="61" t="s">
-        <v>1214</v>
-      </c>
       <c r="L366" s="61" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="M366" s="61" t="s">
         <v>1120</v>
@@ -22786,7 +22749,7 @@
         <v>508</v>
       </c>
       <c r="K367" s="61" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="L367" s="142">
         <v>508</v>
@@ -22891,7 +22854,7 @@
         <v>511</v>
       </c>
       <c r="K370" s="61" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="L370" s="142">
         <v>511</v>
@@ -22951,7 +22914,7 @@
         <v>557</v>
       </c>
       <c r="K372" s="61" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="L372" s="142">
         <v>557</v>
@@ -22960,7 +22923,7 @@
         <v>1120</v>
       </c>
       <c r="N372" s="61" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="O372" s="61"/>
     </row>
@@ -22986,7 +22949,7 @@
         <v>558</v>
       </c>
       <c r="K373" s="61" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="L373" s="142">
         <v>558</v>
@@ -22995,7 +22958,7 @@
         <v>1120</v>
       </c>
       <c r="N373" s="61" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="O373" s="61"/>
     </row>
@@ -23278,9 +23241,7 @@
       <c r="E385" s="61" t="s">
         <v>1119</v>
       </c>
-      <c r="F385" s="61" t="s">
-        <v>1178</v>
-      </c>
+      <c r="F385" s="61"/>
       <c r="G385" s="61"/>
       <c r="H385" s="24"/>
       <c r="I385" s="72"/>
@@ -23297,7 +23258,7 @@
         <v>628</v>
       </c>
       <c r="C386" s="61" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="D386" s="142">
         <v>628</v>
@@ -23306,7 +23267,7 @@
         <v>1119</v>
       </c>
       <c r="F386" s="61" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="G386" s="61"/>
       <c r="H386" s="24"/>
@@ -23324,7 +23285,7 @@
         <v>630</v>
       </c>
       <c r="C387" s="61" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D387" s="142">
         <v>630</v>
@@ -23333,7 +23294,7 @@
         <v>1119</v>
       </c>
       <c r="F387" s="61" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="G387" s="61"/>
       <c r="H387" s="24"/>
@@ -23362,7 +23323,7 @@
     </row>
     <row r="389" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A389" s="146" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B389" s="122">
         <v>675</v>
@@ -23377,7 +23338,7 @@
         <v>650</v>
       </c>
       <c r="F389" s="86" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="G389" s="86"/>
       <c r="H389" s="24"/>
@@ -23401,7 +23362,7 @@
         <v>527</v>
       </c>
       <c r="F390" s="86" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="G390" s="86"/>
       <c r="H390" s="3"/>
@@ -23428,7 +23389,7 @@
         <v>502</v>
       </c>
       <c r="F391" s="86" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="G391" s="86"/>
       <c r="H391" s="9"/>
@@ -23455,7 +23416,7 @@
         <v>527</v>
       </c>
       <c r="F392" s="86" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="G392" s="86"/>
       <c r="H392" s="24"/>
@@ -23480,7 +23441,7 @@
         <v>502</v>
       </c>
       <c r="F393" s="86" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="G393" s="86"/>
       <c r="H393" s="24"/>

</xml_diff>